<commit_message>
fix minor bug on deferment handling, add filtering to the chart Amount by Project
</commit_message>
<xml_diff>
--- a/test_input.xlsx
+++ b/test_input.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drszbtms/Projects/talaria/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B084FAD-4786-2F48-B422-B4C62A73DDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B71051-8467-B646-BE6D-D2290C9B1ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="600" windowWidth="28040" windowHeight="15800" xr2:uid="{1970364C-FF00-A140-8C46-AF4E90FAA54C}"/>
+    <workbookView xWindow="28800" yWindow="-18200" windowWidth="51200" windowHeight="28200" xr2:uid="{1970364C-FF00-A140-8C46-AF4E90FAA54C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -166,7 +166,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A24" activeCellId="1" sqref="A1:H1 A24:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>